<commit_message>
Latest df -> control of RT (200 ms, 3 SD) and accuracy (0.5 - chance level)
</commit_message>
<xml_diff>
--- a/RData/data_rt_WPM.xlsx
+++ b/RData/data_rt_WPM.xlsx
@@ -397,10 +397,10 @@
         <v>823.4285714285714</v>
       </c>
       <c r="D2">
-        <v>6.952134847798976</v>
+        <v>-6.952134847798976</v>
       </c>
       <c r="E2">
-        <v>6.763706993474297</v>
+        <v>-6.763706993474297</v>
       </c>
     </row>
     <row r="3">
@@ -416,10 +416,10 @@
         <v>1422.428571428571</v>
       </c>
       <c r="D3">
-        <v>7.491523672377968</v>
+        <v>-7.491523672377968</v>
       </c>
       <c r="E3">
-        <v>7.266677450186068</v>
+        <v>-7.266677450186068</v>
       </c>
     </row>
     <row r="4">
@@ -435,10 +435,10 @@
         <v>450.8571428571428</v>
       </c>
       <c r="D4">
-        <v>6.944249550683315</v>
+        <v>-6.944249550683315</v>
       </c>
       <c r="E4">
-        <v>6.690757454113832</v>
+        <v>-6.690757454113832</v>
       </c>
     </row>
     <row r="5">
@@ -454,10 +454,10 @@
         <v>405.5714285714286</v>
       </c>
       <c r="D5">
-        <v>6.983665645428913</v>
+        <v>-6.983665645428913</v>
       </c>
       <c r="E5">
-        <v>6.615061042242265</v>
+        <v>-6.615061042242265</v>
       </c>
     </row>
     <row r="6">
@@ -473,10 +473,10 @@
         <v>202.7142857142857</v>
       </c>
       <c r="D6">
-        <v>7.445685204605836</v>
+        <v>-7.445685204605836</v>
       </c>
       <c r="E6">
-        <v>7.236088252796229</v>
+        <v>-7.236088252796229</v>
       </c>
     </row>
     <row r="7">
@@ -492,10 +492,10 @@
         <v>275</v>
       </c>
       <c r="D7">
-        <v>7.134052417057448</v>
+        <v>-7.134052417057448</v>
       </c>
       <c r="E7">
-        <v>6.890237464120239</v>
+        <v>-6.890237464120239</v>
       </c>
     </row>
     <row r="8">
@@ -511,10 +511,10 @@
         <v>843.2857142857143</v>
       </c>
       <c r="D8">
-        <v>7.37077782435057</v>
+        <v>-7.37077782435057</v>
       </c>
       <c r="E8">
-        <v>7.07734884343607</v>
+        <v>-7.07734884343607</v>
       </c>
     </row>
     <row r="9">
@@ -530,10 +530,10 @@
         <v>146.2857142857143</v>
       </c>
       <c r="D9">
-        <v>7.303886466951143</v>
+        <v>-7.303886466951143</v>
       </c>
       <c r="E9">
-        <v>7.067693452822782</v>
+        <v>-7.067693452822782</v>
       </c>
     </row>
     <row r="10">
@@ -549,10 +549,10 @@
         <v>162.2857142857143</v>
       </c>
       <c r="D10">
-        <v>6.805810882332174</v>
+        <v>-6.805810882332174</v>
       </c>
       <c r="E10">
-        <v>6.605897715801645</v>
+        <v>-6.605897715801645</v>
       </c>
     </row>
     <row r="11">
@@ -568,10 +568,10 @@
         <v>481.5714285714286</v>
       </c>
       <c r="D11">
-        <v>6.775701373219641</v>
+        <v>-6.775701373219641</v>
       </c>
       <c r="E11">
-        <v>6.728747593379435</v>
+        <v>-6.728747593379435</v>
       </c>
     </row>
     <row r="12">
@@ -587,10 +587,10 @@
         <v>128.5714285714286</v>
       </c>
       <c r="D12">
-        <v>7.073065731772008</v>
+        <v>-7.073065731772008</v>
       </c>
       <c r="E12">
-        <v>6.852687102861595</v>
+        <v>-6.852687102861595</v>
       </c>
     </row>
     <row r="13">
@@ -606,10 +606,10 @@
         <v>131.4285714285714</v>
       </c>
       <c r="D13">
-        <v>6.619916346589006</v>
+        <v>-6.619916346589006</v>
       </c>
       <c r="E13">
-        <v>6.359562371953563</v>
+        <v>-6.359562371953563</v>
       </c>
     </row>
     <row r="14">
@@ -625,10 +625,10 @@
         <v>436.4285714285714</v>
       </c>
       <c r="D14">
-        <v>7.108065594295618</v>
+        <v>-7.108065594295618</v>
       </c>
       <c r="E14">
-        <v>6.926805908185262</v>
+        <v>-6.926805908185262</v>
       </c>
     </row>
     <row r="15">
@@ -644,10 +644,10 @@
         <v>121.5714285714286</v>
       </c>
       <c r="D15">
-        <v>6.76061501976355</v>
+        <v>-6.76061501976355</v>
       </c>
       <c r="E15">
-        <v>6.520351294447536</v>
+        <v>-6.520351294447536</v>
       </c>
     </row>
     <row r="16">
@@ -663,10 +663,10 @@
         <v>308</v>
       </c>
       <c r="D16">
-        <v>7.164798170655073</v>
+        <v>-7.164798170655073</v>
       </c>
       <c r="E16">
-        <v>6.908702028175726</v>
+        <v>-6.908702028175726</v>
       </c>
     </row>
     <row r="17">
@@ -682,10 +682,10 @@
         <v>280.8571428571428</v>
       </c>
       <c r="D17">
-        <v>7.142530907910885</v>
+        <v>-7.142530907910885</v>
       </c>
       <c r="E17">
-        <v>6.856776320252371</v>
+        <v>-6.856776320252371</v>
       </c>
     </row>
     <row r="18">
@@ -701,10 +701,10 @@
         <v>96.71428571428571</v>
       </c>
       <c r="D18">
-        <v>7.063043874340932</v>
+        <v>-7.063043874340932</v>
       </c>
       <c r="E18">
-        <v>6.894160004126092</v>
+        <v>-6.894160004126092</v>
       </c>
     </row>
     <row r="19">
@@ -720,10 +720,10 @@
         <v>107.5714285714286</v>
       </c>
       <c r="D19">
-        <v>7.285010234412315</v>
+        <v>-7.285010234412315</v>
       </c>
       <c r="E19">
-        <v>7.180032388973652</v>
+        <v>-7.180032388973652</v>
       </c>
     </row>
     <row r="20">
@@ -739,10 +739,10 @@
         <v>331.5714285714286</v>
       </c>
       <c r="D20">
-        <v>7.314461508176811</v>
+        <v>-7.314461508176811</v>
       </c>
       <c r="E20">
-        <v>6.998034422000302</v>
+        <v>-6.998034422000302</v>
       </c>
     </row>
     <row r="21">
@@ -758,10 +758,10 @@
         <v>161.7142857142857</v>
       </c>
       <c r="D21">
-        <v>7.094863515715996</v>
+        <v>-7.094863515715996</v>
       </c>
       <c r="E21">
-        <v>6.815110061347994</v>
+        <v>-6.815110061347994</v>
       </c>
     </row>
     <row r="22">
@@ -777,10 +777,10 @@
         <v>229.8571428571429</v>
       </c>
       <c r="D22">
-        <v>7.175726647783138</v>
+        <v>-7.175726647783138</v>
       </c>
       <c r="E22">
-        <v>6.962926249785784</v>
+        <v>-6.962926249785784</v>
       </c>
     </row>
     <row r="23">
@@ -796,10 +796,10 @@
         <v>196.7142857142857</v>
       </c>
       <c r="D23">
-        <v>7.233796984705399</v>
+        <v>-7.233796984705399</v>
       </c>
       <c r="E23">
-        <v>7.023767386392288</v>
+        <v>-7.023767386392288</v>
       </c>
     </row>
     <row r="24">
@@ -815,10 +815,10 @@
         <v>390.1428571428572</v>
       </c>
       <c r="D24">
-        <v>7.095006492801681</v>
+        <v>-7.095006492801681</v>
       </c>
       <c r="E24">
-        <v>6.811300137658439</v>
+        <v>-6.811300137658439</v>
       </c>
     </row>
     <row r="25">
@@ -834,10 +834,10 @@
         <v>137.2857142857143</v>
       </c>
       <c r="D25">
-        <v>6.980222777484832</v>
+        <v>-6.980222777484832</v>
       </c>
       <c r="E25">
-        <v>6.600201373015838</v>
+        <v>-6.600201373015838</v>
       </c>
     </row>
     <row r="26">
@@ -853,10 +853,10 @@
         <v>1061</v>
       </c>
       <c r="D26">
-        <v>6.964743475718091</v>
+        <v>-6.964743475718091</v>
       </c>
       <c r="E26">
-        <v>6.721830803259133</v>
+        <v>-6.721830803259133</v>
       </c>
     </row>
     <row r="27">
@@ -872,10 +872,10 @@
         <v>79.14285714285714</v>
       </c>
       <c r="D27">
-        <v>7.350428595077923</v>
+        <v>-7.350428595077923</v>
       </c>
       <c r="E27">
-        <v>7.121536100276806</v>
+        <v>-7.121536100276806</v>
       </c>
     </row>
     <row r="28">
@@ -891,10 +891,10 @@
         <v>95.85714285714286</v>
       </c>
       <c r="D28">
-        <v>6.851624205190828</v>
+        <v>-6.851624205190828</v>
       </c>
       <c r="E28">
-        <v>6.601919896392465</v>
+        <v>-6.601919896392465</v>
       </c>
     </row>
     <row r="29">
@@ -910,10 +910,10 @@
         <v>78.14285714285714</v>
       </c>
       <c r="D29">
-        <v>7.174472723554255</v>
+        <v>-7.174472723554255</v>
       </c>
       <c r="E29">
-        <v>7.090923215825319</v>
+        <v>-7.090923215825319</v>
       </c>
     </row>
     <row r="30">
@@ -929,10 +929,10 @@
         <v>310.4285714285714</v>
       </c>
       <c r="D30">
-        <v>6.887613275330245</v>
+        <v>-6.887613275330245</v>
       </c>
       <c r="E30">
-        <v>6.739365038820839</v>
+        <v>-6.739365038820839</v>
       </c>
     </row>
     <row r="31">
@@ -948,10 +948,10 @@
         <v>101</v>
       </c>
       <c r="D31">
-        <v>7.057897253003959</v>
+        <v>-7.057897253003959</v>
       </c>
       <c r="E31">
-        <v>6.763107822913732</v>
+        <v>-6.763107822913732</v>
       </c>
     </row>
     <row r="32">
@@ -967,10 +967,10 @@
         <v>123.5714285714286</v>
       </c>
       <c r="D32">
-        <v>6.757428611566764</v>
+        <v>-6.757428611566764</v>
       </c>
       <c r="E32">
-        <v>6.520542084385408</v>
+        <v>-6.520542084385408</v>
       </c>
     </row>
     <row r="33">
@@ -986,10 +986,10 @@
         <v>89.42857142857143</v>
       </c>
       <c r="D33">
-        <v>7.105785129430214</v>
+        <v>-7.105785129430214</v>
       </c>
       <c r="E33">
-        <v>6.916798323139647</v>
+        <v>-6.916798323139647</v>
       </c>
     </row>
     <row r="34">
@@ -1005,10 +1005,10 @@
         <v>509.2857142857143</v>
       </c>
       <c r="D34">
-        <v>7.132671066577243</v>
+        <v>-7.132671066577243</v>
       </c>
       <c r="E34">
-        <v>6.894155137112569</v>
+        <v>-6.894155137112569</v>
       </c>
     </row>
     <row r="35">
@@ -1024,10 +1024,10 @@
         <v>43.28571428571428</v>
       </c>
       <c r="D35">
-        <v>7.058374451406982</v>
+        <v>-7.058374451406982</v>
       </c>
       <c r="E35">
-        <v>6.927850423299475</v>
+        <v>-6.927850423299475</v>
       </c>
     </row>
     <row r="36">
@@ -1043,10 +1043,10 @@
         <v>60.42857142857143</v>
       </c>
       <c r="D36">
-        <v>7.329034119781786</v>
+        <v>-7.329034119781786</v>
       </c>
       <c r="E36">
-        <v>7.176516879949531</v>
+        <v>-7.176516879949531</v>
       </c>
     </row>
     <row r="37">
@@ -1062,10 +1062,10 @@
         <v>34.42857142857143</v>
       </c>
       <c r="D37">
-        <v>7.10087107367483</v>
+        <v>-7.10087107367483</v>
       </c>
       <c r="E37">
-        <v>6.817377855363781</v>
+        <v>-6.817377855363781</v>
       </c>
     </row>
     <row r="38">
@@ -1081,10 +1081,10 @@
         <v>31.71428571428572</v>
       </c>
       <c r="D38">
-        <v>7.476156436258767</v>
+        <v>-7.476156436258767</v>
       </c>
       <c r="E38">
-        <v>7.297347065458592</v>
+        <v>-7.297347065458592</v>
       </c>
     </row>
     <row r="39">
@@ -1100,10 +1100,10 @@
         <v>28.71428571428572</v>
       </c>
       <c r="D39">
-        <v>7.005484569592134</v>
+        <v>-7.005484569592134</v>
       </c>
       <c r="E39">
-        <v>6.807184398752995</v>
+        <v>-6.807184398752995</v>
       </c>
     </row>
     <row r="40">
@@ -1119,10 +1119,10 @@
         <v>337.2857142857143</v>
       </c>
       <c r="D40">
-        <v>7.06640530786078</v>
+        <v>-7.06640530786078</v>
       </c>
       <c r="E40">
-        <v>6.774045665953955</v>
+        <v>-6.774045665953955</v>
       </c>
     </row>
     <row r="41">
@@ -1138,10 +1138,10 @@
         <v>31.28571428571428</v>
       </c>
       <c r="D41">
-        <v>7.165057884849072</v>
+        <v>-7.165057884849072</v>
       </c>
       <c r="E41">
-        <v>7.035865229496709</v>
+        <v>-7.035865229496709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>